<commit_message>
Added TKR in AR230V
- KC130 added
- Mission brief updated
- MDC updated
- kneeboard updated
</commit_message>
<xml_diff>
--- a/DOC/NTTR Reference.xlsx
+++ b/DOC/NTTR Reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Navpoints" sheetId="1" r:id="rId1"/>
@@ -5889,7 +5889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N525"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D510" sqref="D510"/>
     </sheetView>
   </sheetViews>
@@ -12372,8 +12372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
@@ -12636,8 +12636,9 @@
       <c r="G21" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="150" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
DEV - Active Ranges
- DEV Day and Night MIZ
- Added Active Targets in R74C
- Added AR625
</commit_message>
<xml_diff>
--- a/DOC/NTTR Reference.xlsx
+++ b/DOC/NTTR Reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Navpoints" sheetId="1" r:id="rId1"/>
@@ -5890,7 +5890,7 @@
   <dimension ref="A1:N525"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D510" sqref="D510"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
@@ -12372,7 +12372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -12650,7 +12650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>

</xml_diff>